<commit_message>
2 more leetcodes solved
</commit_message>
<xml_diff>
--- a/docs/Index.xlsx
+++ b/docs/Index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Projects\ProjectDSA\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAC6177-F4DF-43E6-A987-13DCA1E78FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CF88E1-A35C-41ED-9085-C3C876824F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="456" windowWidth="23256" windowHeight="12456" xr2:uid="{B7950DC0-5F1E-48EF-9340-8CAB6CE423A3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B7950DC0-5F1E-48EF-9340-8CAB6CE423A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Problems" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
   <si>
     <t>PLATFORM</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Strings, Hashmaps</t>
   </si>
   <si>
-    <t>Arrays, Hashsets</t>
-  </si>
-  <si>
     <t>Medium</t>
   </si>
   <si>
@@ -111,6 +108,54 @@
   </si>
   <si>
     <t>Arrays, Hashmaps, Bucket Sort</t>
+  </si>
+  <si>
+    <t>21/05/2025</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>Could be solved by Max heap or by ascending sort. Can be solved in linear time with bucket sort.</t>
+  </si>
+  <si>
+    <t>Product of Array Except Self</t>
+  </si>
+  <si>
+    <t>Arrays</t>
+  </si>
+  <si>
+    <t>Valid Sudoku</t>
+  </si>
+  <si>
+    <t>23/05/2025</t>
+  </si>
+  <si>
+    <t>Hashmaps, Sets</t>
+  </si>
+  <si>
+    <t>Arrays, Sets</t>
+  </si>
+  <si>
+    <t>Simple in the end.</t>
+  </si>
+  <si>
+    <t>Encode and Decode Strings</t>
+  </si>
+  <si>
+    <t>25/05/2025</t>
+  </si>
+  <si>
+    <t>Lintcode 659</t>
+  </si>
+  <si>
+    <t>Strings, Arrays, Pointers</t>
+  </si>
+  <si>
+    <t>Longest Consecutive Sequence</t>
+  </si>
+  <si>
+    <t>Hard</t>
   </si>
 </sst>
 </file>
@@ -140,18 +185,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -175,9 +214,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -513,26 +554,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758F6333-ADD2-4F62-82FC-3789A0207F8D}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" customWidth="1"/>
-    <col min="4" max="4" width="39.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="36.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" customWidth="1"/>
+    <col min="4" max="4" width="39.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" customWidth="1"/>
+    <col min="9" max="9" width="83.109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -557,8 +599,11 @@
       <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -569,7 +614,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -584,7 +629,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -610,7 +655,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -636,33 +681,33 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="1">
         <v>49</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -670,39 +715,129 @@
         <v>347</v>
       </c>
       <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
         <v>24</v>
       </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>238</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
       <c r="F8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1">
+        <v>271</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
       <c r="F9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1">
+        <v>128</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
       <c r="F10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
         <v>7</v>
       </c>

</xml_diff>